<commit_message>
Made few changes in main
</commit_message>
<xml_diff>
--- a/Final Output.xlsx
+++ b/Final Output.xlsx
@@ -429,21 +429,19 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Cities</t>
+          <t>Hobby</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>99004361</t>
+          <t>99004359</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Salem
- Gulbarga
- Cuttack</t>
+          <t>Gardening</t>
         </is>
       </c>
     </row>

</xml_diff>